<commit_message>
Modify TestDataParser for ignore merge cells(View Title)
</commit_message>
<xml_diff>
--- a/src/test/resources/simple_test_data.xlsx
+++ b/src/test/resources/simple_test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghongjin/Documents/STV/STV-Project/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB8BDCA6-6620-1E46-914C-333526E5499E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE19B54-9E80-B946-B9B8-841B7420723F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="1" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="View1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>component</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>${YEAR}</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Edit</t>
   </si>
 </sst>
 </file>
@@ -214,7 +220,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -226,6 +232,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9A35-BE5A-E64F-9080-864E7183DD30}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -565,25 +574,46 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="B6" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -593,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434019CE-6758-4C4B-A93B-B77D66012F62}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Modify TestDataParser for more precise merged cell checking logic
</commit_message>
<xml_diff>
--- a/src/test/resources/simple_test_data.xlsx
+++ b/src/test/resources/simple_test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghongjin/Documents/STV/STV-Project/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEE19B54-9E80-B946-B9B8-841B7420723F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864FBBEB-E3BD-8741-AEC1-879412C01D71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="View1" sheetId="1" r:id="rId1"/>
@@ -550,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9A35-BE5A-E64F-9080-864E7183DD30}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -605,9 +605,6 @@
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Modify merged row condition of TestParser for new format test data file
</commit_message>
<xml_diff>
--- a/src/test/resources/simple_test_data.xlsx
+++ b/src/test/resources/simple_test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhenghongjin/Documents/STV/STV-Project/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864FBBEB-E3BD-8741-AEC1-879412C01D71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605D66EA-DC30-1444-87E6-393BC47A9250}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
+    <workbookView xWindow="45000" yWindow="920" windowWidth="29240" windowHeight="17860" activeTab="1" xr2:uid="{0FD658B9-5079-5842-BC6B-31727AF6850F}"/>
   </bookViews>
   <sheets>
     <sheet name="View1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <t>component</t>
   </si>
@@ -34,44 +34,129 @@
     <t>tab_list</t>
   </si>
   <si>
-    <t>folder_list</t>
-  </si>
-  <si>
     <t>//*[@class='android.support.v7.app.ActionBar$Tab' and @index='0']</t>
   </si>
   <si>
     <t>xpath</t>
   </si>
   <si>
-    <t>//*[@resource-id='android:id/button1']</t>
-  </si>
-  <si>
-    <t>calendar-ok</t>
-  </si>
-  <si>
-    <t>calendar-pick-date</t>
-  </si>
-  <si>
-    <t>calendar-pick-year</t>
-  </si>
-  <si>
-    <t>variable</t>
-  </si>
-  <si>
-    <r>
-      <t>//*[@class='android.widget.RelativeLayout' and @index='</t>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>input field</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>TaskList1.png</t>
+  </si>
+  <si>
+    <t>tab_due</t>
+  </si>
+  <si>
+    <t>//*[@class='android.support.v7.app.ActionBar$Tab' and @index='1']</t>
+  </si>
+  <si>
+    <t>//*[@class='android.widget.ImageButton']</t>
+  </si>
+  <si>
+    <t>folder</t>
+  </si>
+  <si>
+    <t>quick add</t>
+  </si>
+  <si>
+    <t>QuickAdd.png</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/task_list_spinner']</t>
+  </si>
+  <si>
+    <t>quick_add_options</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@text='</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="14"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>${INDEX}</t>
+      <t>${NAME}</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']</t>
+    </r>
+  </si>
+  <si>
+    <t>quick_add_editText</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='android:id/input']</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>Input field</t>
+  </si>
+  <si>
+    <t>save_task_btn</t>
+  </si>
+  <si>
+    <t>//*[@resource-id='org.dmfs.tasks:id/editor_action_save']</t>
+  </si>
+  <si>
+    <t>EditTask1.png</t>
+  </si>
+  <si>
+    <t>cancel_btn</t>
+  </si>
+  <si>
+    <t>folder_dropdown</t>
+  </si>
+  <si>
+    <t>FolderOptions.png</t>
+  </si>
+  <si>
+    <t>title_editText</t>
+  </si>
+  <si>
+    <t>//*[@index='0' and contains(@class, 'android.widget.EditText')]</t>
+  </si>
+  <si>
+    <t>status_dropdown</t>
+  </si>
+  <si>
+    <t>//*[@index='1' and contains(@class, 'android.widget.Spinner')]</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.TextView' and @text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -81,26 +166,48 @@
     </r>
   </si>
   <si>
-    <t>${INDEX}</t>
-  </si>
-  <si>
-    <t>${TEXT}</t>
-  </si>
-  <si>
-    <r>
-      <t>//*[@class='android.view.View' and @text='</t>
+    <t>quick_add_btn</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@index='</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="14"/>
         <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)_x0000_"/>
       </rPr>
-      <t>${TEXT}</t>
+      <t>${INDEX}</t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>']/android.widget.ImageView[@resource-id='org.dmfs.tasks:id/quick_add_task']</t>
+    </r>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <r>
+      <t>//*[@class='android.widget.LinearLayout' and ./android.widget.TextView[@text='</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)_x0000_"/>
+      </rPr>
+      <t>${NAME}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
@@ -110,43 +217,17 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>//*[@class='android.widget.TextView' and @text='</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri (Body)_x0000_"/>
-      </rPr>
-      <t>${YEAR}</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>']</t>
-    </r>
-  </si>
-  <si>
-    <t>${YEAR}</t>
-  </si>
-  <si>
-    <t>Main</t>
-  </si>
-  <si>
-    <t>Edit</t>
+    <t>${NAME}</t>
+  </si>
+  <si>
+    <t>${INDEX}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,20 +236,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="14"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)_x0000_"/>
     </font>
     <font>
       <sz val="14"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -182,7 +284,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -216,28 +318,110 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{296F9A35-BE5A-E64F-9080-864E7183DD30}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -562,55 +746,132 @@
     <col min="2" max="2" width="108.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="33" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="19">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19">
+      <c r="A3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="6" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="17"/>
+    </row>
+    <row r="4" spans="1:5" ht="19">
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="17"/>
+    </row>
+    <row r="5" spans="1:5" ht="19">
+      <c r="A5" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" spans="1:5" ht="19">
+      <c r="A6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="18"/>
+    </row>
+    <row r="7" spans="1:5" ht="19">
+      <c r="A7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" ht="19">
+      <c r="A8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="6" t="s">
+      <c r="C8" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="19">
+      <c r="A9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
+      <c r="B9" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A5:C5"/>
+  <mergeCells count="3">
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="E2:E6"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E2:E6" r:id="rId1" display="TaskList1.png" xr:uid="{4F4AC58C-2ED9-E944-B980-3B82E00E69AC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -618,60 +879,124 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434019CE-6758-4C4B-A93B-B77D66012F62}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="108.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="33" customHeight="1">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="33" customHeight="1">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="19">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19">
+      <c r="A3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" ht="19">
+      <c r="A4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" ht="19">
+      <c r="A5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19">
+      <c r="A6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="19">
+      <c r="A7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="17"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E6:E7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E2:E4" r:id="rId1" display="EditTask1.png" xr:uid="{7DCE6EA1-57AC-2C41-959F-AEACBBC57B30}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{16D0B242-1500-AC4B-9C0D-4FF421AA5AFF}"/>
+    <hyperlink ref="E6:E7" r:id="rId3" display="EditTask1.png" xr:uid="{A07C543E-42CF-DA4D-8629-5AF877AC3C4F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>